<commit_message>
Atualização automática de CAXIAS_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/CAXIAS_DO_SUL.xlsx
+++ b/CAXIAS_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B712698B-D8E2-49CD-9CE3-EBDAC8CC469A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E45AFE6B-2835-4361-B2C1-56DCEAA4AC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1332,7 +1319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1393,30 +1380,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1434,7 +1397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1473,17 +1436,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1529,7 +1487,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{875FD3EF-9A48-42AE-BB67-14813CFEB3B3}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{E975784B-9B5D-48A4-A2EF-DC30491A3086}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1559,10 +1517,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDD5CBDD-8A10-49B1-8147-9DEC92B3418C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83C9F84E-96A8-4422-8258-A46FA4DC29ED}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1600,7 +1558,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{822D8380-3EC3-45AA-9624-AE8F3434000B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74AD3176-53B9-41E8-8C41-79F7FF76505D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1663,7 +1621,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B570A0A5-F345-4302-AFBF-D525D3A84A9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C832785-7BFD-4B04-854A-1CDB84D87D4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1682,7 +1640,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCFCB021-FA9F-B101-D231-03B0131E0700}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3372A19E-3B27-BEB6-A67E-265917941DC3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1731,7 +1689,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2B8B27-3E5F-1961-1D5A-1998291AD438}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6EC0752-EC52-BDF8-6CA2-825292B7DDFC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1750,7 +1708,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57702E22-6BEC-36F0-389B-E041130F938A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A05DE9-9E1B-84B0-3863-C234E641F5C6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1781,7 +1739,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E78079-5D06-7F69-2C62-F7B6BB0EBAE4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5170F9BA-7DAC-2ABC-2AB2-79401BF3FD35}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1812,7 +1770,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7F2B47B-4E6B-025E-E02C-30FACE879D60}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A0EA8D-D7AC-E593-40FE-ABB672641D5A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1855,7 +1813,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A70D15-5076-4697-AC15-AAD6D36E9D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{130E44C8-F1B6-4CAE-A7C8-3C572CF55E27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,7 +1851,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52554E79-B6B8-4A30-9854-062007ABCFEE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8E0D6BF-D36C-4C4D-BD8A-42CECBCDFC32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +1894,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D65AE268-AC55-4A61-90C0-8CC76E8B9720}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA52C176-9007-4183-A498-D0D2EA9D05A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2249,7 +2207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443BB890-49E7-4116-8E6F-55F8FEEC0125}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25398D57-92BC-4937-AD08-4973AB951220}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2261,98 +2219,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5586,19 +5544,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5632,46 +5590,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5679,7 +5637,7 @@
       <c r="A2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>175395</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5691,10 +5649,10 @@
       <c r="E2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>7.39</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>73.900000000000006</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5723,7 +5681,7 @@
       <c r="A3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>193860</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5735,10 +5693,10 @@
       <c r="E3" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>8.5</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>85</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5767,7 +5725,7 @@
       <c r="A4" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>366966</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5779,10 +5737,10 @@
       <c r="E4" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>8.5</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>85</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5811,7 +5769,7 @@
       <c r="A5" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>193862</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5823,10 +5781,10 @@
       <c r="E5" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>8.5</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>85</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5855,7 +5813,7 @@
       <c r="A6" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>4439</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5867,10 +5825,10 @@
       <c r="E6" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>11.62</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>116.2</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5899,7 +5857,7 @@
       <c r="A7" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>4814</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5911,10 +5869,10 @@
       <c r="E7" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>5.2</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>52</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5943,7 +5901,7 @@
       <c r="A8" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>5241</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5955,10 +5913,10 @@
       <c r="E8" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>11.62</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>116.2</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5987,7 +5945,7 @@
       <c r="A9" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>152160</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5999,10 +5957,10 @@
       <c r="E9" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>7.2</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>72</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -6031,7 +5989,7 @@
       <c r="A10" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>198001</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6043,10 +6001,10 @@
       <c r="E10" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>19.5</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>195</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -6075,7 +6033,7 @@
       <c r="A11" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>191668</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6087,10 +6045,10 @@
       <c r="E11" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>14.9</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>148.96</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6119,7 +6077,7 @@
       <c r="A12" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>204941</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6131,10 +6089,10 @@
       <c r="E12" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>14.9</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>148.96</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6163,7 +6121,7 @@
       <c r="A13" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>259257</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6175,10 +6133,10 @@
       <c r="E13" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>18.5</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>185</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6207,7 +6165,7 @@
       <c r="A14" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>277341</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6219,10 +6177,10 @@
       <c r="E14" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>19.5</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>195</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6251,7 +6209,7 @@
       <c r="A15" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>298828</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6263,10 +6221,10 @@
       <c r="E15" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>19.5</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>195</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -6295,7 +6253,7 @@
       <c r="A16" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>375050</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6307,10 +6265,10 @@
       <c r="E16" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>55.57</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -6339,7 +6297,7 @@
       <c r="A17" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>388807</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6351,10 +6309,10 @@
       <c r="E17" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>43.08</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>430.8</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -6383,7 +6341,7 @@
       <c r="A18" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>388891</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6395,10 +6353,10 @@
       <c r="E18" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>52.57</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>525.70000000000005</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -6427,7 +6385,7 @@
       <c r="A19" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>390479</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -6439,10 +6397,10 @@
       <c r="E19" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="20">
         <v>55.57</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -6471,7 +6429,7 @@
       <c r="A20" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="19">
         <v>390523</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -6483,10 +6441,10 @@
       <c r="E20" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>55.57</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -6515,7 +6473,7 @@
       <c r="A21" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>390526</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6527,10 +6485,10 @@
       <c r="E21" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="20">
         <v>55.57</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -6559,7 +6517,7 @@
       <c r="A22" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>390529</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -6571,10 +6529,10 @@
       <c r="E22" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>55.57</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -6603,7 +6561,7 @@
       <c r="A23" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="19">
         <v>390533</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -6615,10 +6573,10 @@
       <c r="E23" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="20">
         <v>55.57</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -6647,7 +6605,7 @@
       <c r="A24" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="19">
         <v>390599</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -6659,10 +6617,10 @@
       <c r="E24" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>55.57</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -6691,7 +6649,7 @@
       <c r="A25" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="19">
         <v>390610</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6703,10 +6661,10 @@
       <c r="E25" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="20">
         <v>55.57</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -6735,7 +6693,7 @@
       <c r="A26" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="19">
         <v>390635</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -6747,10 +6705,10 @@
       <c r="E26" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="20">
         <v>55.57</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -6779,7 +6737,7 @@
       <c r="A27" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="19">
         <v>390638</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -6791,10 +6749,10 @@
       <c r="E27" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="20">
         <v>55.57</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="20">
         <v>555.70000000000005</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -6823,7 +6781,7 @@
       <c r="A28" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="19">
         <v>399962</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -6835,10 +6793,10 @@
       <c r="E28" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <v>29.4</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="20">
         <v>294</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -6867,7 +6825,7 @@
       <c r="A29" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="19">
         <v>406833</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -6879,10 +6837,10 @@
       <c r="E29" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="20">
         <v>53.24</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="20">
         <v>532.35</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -6911,7 +6869,7 @@
       <c r="A30" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="19">
         <v>410099</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -6923,10 +6881,10 @@
       <c r="E30" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="20">
         <v>56.1</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="20">
         <v>561</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -6955,7 +6913,7 @@
       <c r="A31" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="19">
         <v>417381</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -6967,10 +6925,10 @@
       <c r="E31" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="20">
         <v>56.1</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="20">
         <v>561</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -6999,7 +6957,7 @@
       <c r="A32" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="19">
         <v>425638</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -7011,10 +6969,10 @@
       <c r="E32" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <v>45.68</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="20">
         <v>456.75</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -7043,7 +7001,7 @@
       <c r="A33" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="19">
         <v>426032</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -7055,10 +7013,10 @@
       <c r="E33" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="20">
         <v>45.68</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="20">
         <v>456.75</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -7087,7 +7045,7 @@
       <c r="A34" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="19">
         <v>426044</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -7099,10 +7057,10 @@
       <c r="E34" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="20">
         <v>45.68</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="20">
         <v>456.75</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -7131,7 +7089,7 @@
       <c r="A35" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="19">
         <v>452294</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -7143,10 +7101,10 @@
       <c r="E35" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <v>1789.3</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <v>2105</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -7175,7 +7133,7 @@
       <c r="A36" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="19">
         <v>452368</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -7187,10 +7145,10 @@
       <c r="E36" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="20">
         <v>1557.32</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="20">
         <v>1670</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -7219,7 +7177,7 @@
       <c r="A37" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="19">
         <v>452369</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -7231,10 +7189,10 @@
       <c r="E37" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="20">
         <v>1059.4100000000001</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="20">
         <v>1136.0899999999999</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -7263,7 +7221,7 @@
       <c r="A38" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="19">
         <v>452370</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -7275,10 +7233,10 @@
       <c r="E38" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="20">
         <v>680.49</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="20">
         <v>786.69</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -7307,7 +7265,7 @@
       <c r="A39" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="19">
         <v>452371</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -7319,10 +7277,10 @@
       <c r="E39" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="20">
         <v>680.49</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="20">
         <v>786.69</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -7351,7 +7309,7 @@
       <c r="A40" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="19">
         <v>452372</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -7363,10 +7321,10 @@
       <c r="E40" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <v>372.09</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="20">
         <v>399</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -7395,7 +7353,7 @@
       <c r="A41" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B41" s="19">
         <v>452373</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -7407,10 +7365,10 @@
       <c r="E41" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <v>322.47000000000003</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="20">
         <v>342.99</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -7439,7 +7397,7 @@
       <c r="A42" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="19">
         <v>582136</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -7451,10 +7409,10 @@
       <c r="E42" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <v>565</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="20">
         <v>565</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -7483,7 +7441,7 @@
       <c r="A43" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="19">
         <v>582137</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -7495,10 +7453,10 @@
       <c r="E43" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <v>4700</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="20">
         <v>4700</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -7527,7 +7485,7 @@
       <c r="A44" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="19">
         <v>582138</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -7539,10 +7497,10 @@
       <c r="E44" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <v>3900</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="20">
         <v>3900</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -7571,7 +7529,7 @@
       <c r="A45" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="19">
         <v>582139</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -7583,10 +7541,10 @@
       <c r="E45" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="20">
         <v>2800</v>
       </c>
-      <c r="G45" s="23">
+      <c r="G45" s="20">
         <v>2800</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -7625,14 +7583,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>355</v>
       </c>
     </row>
@@ -7663,112 +7621,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>361</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7793,54 +7751,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>370</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>372</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>374</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>380</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>381</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>383</v>
       </c>
     </row>
@@ -7851,41 +7810,41 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45931</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>114474</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>15921</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>387</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>387</v>
       </c>
     </row>
@@ -7916,25 +7875,24 @@
       <c r="B1" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>389</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="35">
         <v>309</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="B2" s="38">
-        <v>309</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>2.0433805052241769E-2</v>
       </c>
     </row>

</xml_diff>